<commit_message>
Updated Elsweyr sets w/o setId and w/o zoneId
</commit_message>
<xml_diff>
--- a/LibSets/2019-05-13_LibSets_SetData.xlsx
+++ b/LibSets/2019-05-13_LibSets_SetData.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4120" uniqueCount="2562">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4178" uniqueCount="2574">
   <si>
     <t>Balorgh</t>
   </si>
@@ -7695,9 +7695,6 @@
     <t>Sunspire</t>
   </si>
   <si>
-    <t>Sonnen?</t>
-  </si>
-  <si>
     <t>?</t>
   </si>
   <si>
@@ -7710,9 +7707,6 @@
     <t>TODO: Add Elsyweyr zone Ids</t>
   </si>
   <si>
-    <t>Sonnenturm</t>
-  </si>
-  <si>
     <t>Crafty Alfiq</t>
   </si>
   <si>
@@ -7723,6 +7717,48 @@
   </si>
   <si>
     <t>Overland</t>
+  </si>
+  <si>
+    <t>Senche-raht's Grit</t>
+  </si>
+  <si>
+    <t>Vastarie's Tutelage</t>
+  </si>
+  <si>
+    <t>Coldharbour's Favorite</t>
+  </si>
+  <si>
+    <t>Crafted</t>
+  </si>
+  <si>
+    <t>Sonnspitz</t>
+  </si>
+  <si>
+    <t>False God's Devotion</t>
+  </si>
+  <si>
+    <t>Eye of Nahviintaas</t>
+  </si>
+  <si>
+    <t>Tooth of Lokkestiiz</t>
+  </si>
+  <si>
+    <t>Claw of Yolnakhriin</t>
+  </si>
+  <si>
+    <t>Perfected False God's Devotion</t>
+  </si>
+  <si>
+    <t>Perfected Tooth of Lokkestiiz</t>
+  </si>
+  <si>
+    <t>Perfected Eye of Nahviintaas</t>
+  </si>
+  <si>
+    <t>Perfected Claw of Yolnakhriin</t>
+  </si>
+  <si>
+    <t>Trial</t>
   </si>
 </sst>
 </file>
@@ -8250,10 +8286,10 @@
   <dimension ref="A1:AC486"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="AA373" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="R396" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AB382" sqref="AB382"/>
+      <selection pane="bottomRight" activeCell="W422" sqref="W422"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38783,10 +38819,10 @@
     </row>
     <row r="409" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C409" t="s">
-        <v>2558</v>
+        <v>2556</v>
       </c>
       <c r="I409" t="s">
-        <v>2561</v>
+        <v>2559</v>
       </c>
       <c r="K409" t="s">
         <v>105</v>
@@ -38834,10 +38870,10 @@
     </row>
     <row r="410" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C410" t="s">
+        <v>2557</v>
+      </c>
+      <c r="I410" t="s">
         <v>2559</v>
-      </c>
-      <c r="I410" t="s">
-        <v>2561</v>
       </c>
       <c r="K410" t="s">
         <v>105</v>
@@ -38885,10 +38921,10 @@
     </row>
     <row r="411" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C411" t="s">
-        <v>2560</v>
+        <v>2558</v>
       </c>
       <c r="I411" t="s">
-        <v>2561</v>
+        <v>2559</v>
       </c>
       <c r="K411" t="s">
         <v>105</v>
@@ -38935,13 +38971,34 @@
       </c>
     </row>
     <row r="412" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="C412" t="s">
+        <v>2560</v>
+      </c>
+      <c r="I412" t="s">
+        <v>2563</v>
+      </c>
+      <c r="K412" t="s">
+        <v>105</v>
+      </c>
+      <c r="L412" t="s">
+        <v>105</v>
+      </c>
+      <c r="P412" t="s">
+        <v>2552</v>
+      </c>
       <c r="Q412" s="3" t="str">
         <f>IF(R412&lt;&gt;"",VLOOKUP(R412,'ESO zone constants'!$E$3:$J$1002,5,FALSE),"")</f>
         <v/>
       </c>
+      <c r="R412" s="3" t="s">
+        <v>1395</v>
+      </c>
+      <c r="W412" s="3">
+        <v>14</v>
+      </c>
       <c r="X412" t="str">
         <f>VLOOKUP(W412,'LibSets constants'!$A$2:$B$16,2,FALSE)</f>
-        <v>Included in base game</v>
+        <v>Elsweyr</v>
       </c>
       <c r="Y412" s="7" t="str">
         <f t="shared" si="30"/>
@@ -38957,7 +39014,7 @@
       </c>
       <c r="AB412" s="7" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v xml:space="preserve"> --Senche-raht's Grit / </v>
       </c>
       <c r="AC412" s="7" t="str">
         <f t="shared" si="34"/>
@@ -38965,13 +39022,34 @@
       </c>
     </row>
     <row r="413" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="C413" t="s">
+        <v>2561</v>
+      </c>
+      <c r="I413" t="s">
+        <v>2563</v>
+      </c>
+      <c r="K413" t="s">
+        <v>105</v>
+      </c>
+      <c r="L413" t="s">
+        <v>105</v>
+      </c>
+      <c r="P413" t="s">
+        <v>2552</v>
+      </c>
       <c r="Q413" s="3" t="str">
         <f>IF(R413&lt;&gt;"",VLOOKUP(R413,'ESO zone constants'!$E$3:$J$1002,5,FALSE),"")</f>
         <v/>
       </c>
+      <c r="R413" s="3" t="s">
+        <v>1395</v>
+      </c>
+      <c r="W413" s="3">
+        <v>14</v>
+      </c>
       <c r="X413" t="str">
         <f>VLOOKUP(W413,'LibSets constants'!$A$2:$B$16,2,FALSE)</f>
-        <v>Included in base game</v>
+        <v>Elsweyr</v>
       </c>
       <c r="Y413" s="7" t="str">
         <f t="shared" si="30"/>
@@ -38987,7 +39065,7 @@
       </c>
       <c r="AB413" s="7" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v xml:space="preserve"> --Vastarie's Tutelage / </v>
       </c>
       <c r="AC413" s="7" t="str">
         <f t="shared" si="34"/>
@@ -38995,13 +39073,34 @@
       </c>
     </row>
     <row r="414" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="C414" t="s">
+        <v>2562</v>
+      </c>
+      <c r="I414" t="s">
+        <v>2563</v>
+      </c>
+      <c r="K414" t="s">
+        <v>105</v>
+      </c>
+      <c r="L414" t="s">
+        <v>105</v>
+      </c>
+      <c r="P414" t="s">
+        <v>2552</v>
+      </c>
       <c r="Q414" s="3" t="str">
         <f>IF(R414&lt;&gt;"",VLOOKUP(R414,'ESO zone constants'!$E$3:$J$1002,5,FALSE),"")</f>
         <v/>
       </c>
+      <c r="R414" s="3" t="s">
+        <v>1395</v>
+      </c>
+      <c r="W414" s="3">
+        <v>14</v>
+      </c>
       <c r="X414" t="str">
         <f>VLOOKUP(W414,'LibSets constants'!$A$2:$B$16,2,FALSE)</f>
-        <v>Included in base game</v>
+        <v>Elsweyr</v>
       </c>
       <c r="Y414" s="7" t="str">
         <f t="shared" si="30"/>
@@ -39017,7 +39116,7 @@
       </c>
       <c r="AB414" s="7" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v xml:space="preserve"> --Coldharbour's Favorite / </v>
       </c>
       <c r="AC414" s="7" t="str">
         <f t="shared" si="34"/>
@@ -39025,13 +39124,31 @@
       </c>
     </row>
     <row r="415" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="C415" t="s">
+        <v>2565</v>
+      </c>
+      <c r="I415" t="s">
+        <v>2573</v>
+      </c>
+      <c r="K415" t="s">
+        <v>105</v>
+      </c>
+      <c r="L415" t="s">
+        <v>105</v>
+      </c>
       <c r="Q415" s="3" t="str">
         <f>IF(R415&lt;&gt;"",VLOOKUP(R415,'ESO zone constants'!$E$3:$J$1002,5,FALSE),"")</f>
         <v/>
       </c>
+      <c r="R415" s="3" t="s">
+        <v>2551</v>
+      </c>
+      <c r="W415" s="3">
+        <v>14</v>
+      </c>
       <c r="X415" t="str">
         <f>VLOOKUP(W415,'LibSets constants'!$A$2:$B$16,2,FALSE)</f>
-        <v>Included in base game</v>
+        <v>Elsweyr</v>
       </c>
       <c r="Y415" s="7" t="str">
         <f t="shared" si="30"/>
@@ -39047,7 +39164,7 @@
       </c>
       <c r="AB415" s="7" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v xml:space="preserve"> --False God's Devotion / </v>
       </c>
       <c r="AC415" s="7" t="str">
         <f t="shared" si="34"/>
@@ -39055,13 +39172,31 @@
       </c>
     </row>
     <row r="416" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="C416" t="s">
+        <v>2566</v>
+      </c>
+      <c r="I416" t="s">
+        <v>2573</v>
+      </c>
+      <c r="K416" t="s">
+        <v>105</v>
+      </c>
+      <c r="L416" t="s">
+        <v>105</v>
+      </c>
       <c r="Q416" s="3" t="str">
         <f>IF(R416&lt;&gt;"",VLOOKUP(R416,'ESO zone constants'!$E$3:$J$1002,5,FALSE),"")</f>
         <v/>
       </c>
+      <c r="R416" s="3" t="s">
+        <v>2551</v>
+      </c>
+      <c r="W416" s="3">
+        <v>14</v>
+      </c>
       <c r="X416" t="str">
         <f>VLOOKUP(W416,'LibSets constants'!$A$2:$B$16,2,FALSE)</f>
-        <v>Included in base game</v>
+        <v>Elsweyr</v>
       </c>
       <c r="Y416" s="7" t="str">
         <f t="shared" si="30"/>
@@ -39077,21 +39212,39 @@
       </c>
       <c r="AB416" s="7" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v xml:space="preserve"> --Eye of Nahviintaas / </v>
       </c>
       <c r="AC416" s="7" t="str">
         <f t="shared" si="34"/>
         <v/>
       </c>
     </row>
-    <row r="417" spans="17:29" x14ac:dyDescent="0.25">
+    <row r="417" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C417" t="s">
+        <v>2567</v>
+      </c>
+      <c r="I417" t="s">
+        <v>2573</v>
+      </c>
+      <c r="K417" t="s">
+        <v>105</v>
+      </c>
+      <c r="L417" t="s">
+        <v>105</v>
+      </c>
       <c r="Q417" s="3" t="str">
         <f>IF(R417&lt;&gt;"",VLOOKUP(R417,'ESO zone constants'!$E$3:$J$1002,5,FALSE),"")</f>
         <v/>
       </c>
+      <c r="R417" s="3" t="s">
+        <v>2551</v>
+      </c>
+      <c r="W417" s="3">
+        <v>14</v>
+      </c>
       <c r="X417" t="str">
         <f>VLOOKUP(W417,'LibSets constants'!$A$2:$B$16,2,FALSE)</f>
-        <v>Included in base game</v>
+        <v>Elsweyr</v>
       </c>
       <c r="Y417" s="7" t="str">
         <f t="shared" si="30"/>
@@ -39107,17 +39260,39 @@
       </c>
       <c r="AB417" s="7" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v xml:space="preserve"> --Tooth of Lokkestiiz / </v>
       </c>
       <c r="AC417" s="7" t="str">
         <f t="shared" si="34"/>
         <v/>
       </c>
     </row>
-    <row r="418" spans="17:29" x14ac:dyDescent="0.25">
+    <row r="418" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C418" t="s">
+        <v>2568</v>
+      </c>
+      <c r="I418" t="s">
+        <v>2573</v>
+      </c>
+      <c r="K418" t="s">
+        <v>105</v>
+      </c>
+      <c r="L418" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q418" s="3" t="str">
+        <f>IF(R418&lt;&gt;"",VLOOKUP(R418,'ESO zone constants'!$E$3:$J$1002,5,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R418" s="3" t="s">
+        <v>2551</v>
+      </c>
+      <c r="W418" s="3">
+        <v>14</v>
+      </c>
       <c r="X418" t="str">
         <f>VLOOKUP(W418,'LibSets constants'!$A$2:$B$16,2,FALSE)</f>
-        <v>Included in base game</v>
+        <v>Elsweyr</v>
       </c>
       <c r="Y418" s="7" t="str">
         <f t="shared" si="30"/>
@@ -39133,17 +39308,39 @@
       </c>
       <c r="AB418" s="7" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v xml:space="preserve"> --Claw of Yolnakhriin / </v>
       </c>
       <c r="AC418" s="7" t="str">
         <f t="shared" si="34"/>
         <v/>
       </c>
     </row>
-    <row r="419" spans="17:29" x14ac:dyDescent="0.25">
+    <row r="419" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C419" t="s">
+        <v>2569</v>
+      </c>
+      <c r="I419" t="s">
+        <v>2573</v>
+      </c>
+      <c r="K419" t="s">
+        <v>106</v>
+      </c>
+      <c r="L419" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q419" s="3" t="str">
+        <f>IF(R419&lt;&gt;"",VLOOKUP(R419,'ESO zone constants'!$E$3:$J$1002,5,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R419" s="3" t="s">
+        <v>2551</v>
+      </c>
+      <c r="W419" s="3">
+        <v>14</v>
+      </c>
       <c r="X419" t="str">
         <f>VLOOKUP(W419,'LibSets constants'!$A$2:$B$16,2,FALSE)</f>
-        <v>Included in base game</v>
+        <v>Elsweyr</v>
       </c>
       <c r="Y419" s="7" t="str">
         <f t="shared" si="30"/>
@@ -39159,17 +39356,39 @@
       </c>
       <c r="AB419" s="7" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v xml:space="preserve"> --Perfected False God's Devotion / </v>
       </c>
       <c r="AC419" s="7" t="str">
         <f t="shared" si="34"/>
         <v/>
       </c>
     </row>
-    <row r="420" spans="17:29" x14ac:dyDescent="0.25">
+    <row r="420" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C420" t="s">
+        <v>2570</v>
+      </c>
+      <c r="I420" t="s">
+        <v>2573</v>
+      </c>
+      <c r="K420" t="s">
+        <v>106</v>
+      </c>
+      <c r="L420" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q420" s="3" t="str">
+        <f>IF(R420&lt;&gt;"",VLOOKUP(R420,'ESO zone constants'!$E$3:$J$1002,5,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R420" s="3" t="s">
+        <v>2551</v>
+      </c>
+      <c r="W420" s="3">
+        <v>14</v>
+      </c>
       <c r="X420" t="str">
         <f>VLOOKUP(W420,'LibSets constants'!$A$2:$B$16,2,FALSE)</f>
-        <v>Included in base game</v>
+        <v>Elsweyr</v>
       </c>
       <c r="Y420" s="7" t="str">
         <f t="shared" si="30"/>
@@ -39185,17 +39404,39 @@
       </c>
       <c r="AB420" s="7" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v xml:space="preserve"> --Perfected Tooth of Lokkestiiz / </v>
       </c>
       <c r="AC420" s="7" t="str">
         <f t="shared" si="34"/>
         <v/>
       </c>
     </row>
-    <row r="421" spans="17:29" x14ac:dyDescent="0.25">
+    <row r="421" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C421" t="s">
+        <v>2571</v>
+      </c>
+      <c r="I421" t="s">
+        <v>2573</v>
+      </c>
+      <c r="K421" t="s">
+        <v>106</v>
+      </c>
+      <c r="L421" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q421" s="3" t="str">
+        <f>IF(R421&lt;&gt;"",VLOOKUP(R421,'ESO zone constants'!$E$3:$J$1002,5,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R421" s="3" t="s">
+        <v>2551</v>
+      </c>
+      <c r="W421" s="3">
+        <v>14</v>
+      </c>
       <c r="X421" t="str">
         <f>VLOOKUP(W421,'LibSets constants'!$A$2:$B$16,2,FALSE)</f>
-        <v>Included in base game</v>
+        <v>Elsweyr</v>
       </c>
       <c r="Y421" s="7" t="str">
         <f t="shared" si="30"/>
@@ -39211,17 +39452,39 @@
       </c>
       <c r="AB421" s="7" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v xml:space="preserve"> --Perfected Eye of Nahviintaas / </v>
       </c>
       <c r="AC421" s="7" t="str">
         <f t="shared" si="34"/>
         <v/>
       </c>
     </row>
-    <row r="422" spans="17:29" x14ac:dyDescent="0.25">
+    <row r="422" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C422" t="s">
+        <v>2572</v>
+      </c>
+      <c r="I422" t="s">
+        <v>2573</v>
+      </c>
+      <c r="K422" t="s">
+        <v>106</v>
+      </c>
+      <c r="L422" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q422" s="3" t="str">
+        <f>IF(R422&lt;&gt;"",VLOOKUP(R422,'ESO zone constants'!$E$3:$J$1002,5,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R422" s="3" t="s">
+        <v>2551</v>
+      </c>
+      <c r="W422" s="3">
+        <v>14</v>
+      </c>
       <c r="X422" t="str">
         <f>VLOOKUP(W422,'LibSets constants'!$A$2:$B$16,2,FALSE)</f>
-        <v>Included in base game</v>
+        <v>Elsweyr</v>
       </c>
       <c r="Y422" s="7" t="str">
         <f t="shared" si="30"/>
@@ -39237,14 +39500,18 @@
       </c>
       <c r="AB422" s="7" t="str">
         <f t="shared" si="33"/>
-        <v/>
+        <v xml:space="preserve"> --Perfected Claw of Yolnakhriin / </v>
       </c>
       <c r="AC422" s="7" t="str">
         <f t="shared" si="34"/>
         <v/>
       </c>
     </row>
-    <row r="423" spans="17:29" x14ac:dyDescent="0.25">
+    <row r="423" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="Q423" s="3" t="str">
+        <f>IF(R423&lt;&gt;"",VLOOKUP(R423,'ESO zone constants'!$E$3:$J$1002,5,FALSE),"")</f>
+        <v/>
+      </c>
       <c r="Y423" s="7" t="str">
         <f t="shared" si="30"/>
         <v/>
@@ -39266,7 +39533,11 @@
         <v/>
       </c>
     </row>
-    <row r="424" spans="17:29" x14ac:dyDescent="0.25">
+    <row r="424" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="Q424" s="3" t="str">
+        <f>IF(R424&lt;&gt;"",VLOOKUP(R424,'ESO zone constants'!$E$3:$J$1002,5,FALSE),"")</f>
+        <v/>
+      </c>
       <c r="Y424" s="7" t="str">
         <f t="shared" si="30"/>
         <v/>
@@ -39288,7 +39559,11 @@
         <v/>
       </c>
     </row>
-    <row r="425" spans="17:29" x14ac:dyDescent="0.25">
+    <row r="425" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="Q425" s="3" t="str">
+        <f>IF(R425&lt;&gt;"",VLOOKUP(R425,'ESO zone constants'!$E$3:$J$1002,5,FALSE),"")</f>
+        <v/>
+      </c>
       <c r="Y425" s="7" t="str">
         <f t="shared" si="30"/>
         <v/>
@@ -39310,7 +39585,11 @@
         <v/>
       </c>
     </row>
-    <row r="426" spans="17:29" x14ac:dyDescent="0.25">
+    <row r="426" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="Q426" s="3" t="str">
+        <f>IF(R426&lt;&gt;"",VLOOKUP(R426,'ESO zone constants'!$E$3:$J$1002,5,FALSE),"")</f>
+        <v/>
+      </c>
       <c r="Y426" s="7" t="str">
         <f t="shared" si="30"/>
         <v/>
@@ -39332,7 +39611,11 @@
         <v/>
       </c>
     </row>
-    <row r="427" spans="17:29" x14ac:dyDescent="0.25">
+    <row r="427" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="Q427" s="3" t="str">
+        <f>IF(R427&lt;&gt;"",VLOOKUP(R427,'ESO zone constants'!$E$3:$J$1002,5,FALSE),"")</f>
+        <v/>
+      </c>
       <c r="Y427" s="7" t="str">
         <f t="shared" si="30"/>
         <v/>
@@ -39354,7 +39637,11 @@
         <v/>
       </c>
     </row>
-    <row r="428" spans="17:29" x14ac:dyDescent="0.25">
+    <row r="428" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="Q428" s="3" t="str">
+        <f>IF(R428&lt;&gt;"",VLOOKUP(R428,'ESO zone constants'!$E$3:$J$1002,5,FALSE),"")</f>
+        <v/>
+      </c>
       <c r="Y428" s="7" t="str">
         <f t="shared" si="30"/>
         <v/>
@@ -39376,7 +39663,11 @@
         <v/>
       </c>
     </row>
-    <row r="429" spans="17:29" x14ac:dyDescent="0.25">
+    <row r="429" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="Q429" s="3" t="str">
+        <f>IF(R429&lt;&gt;"",VLOOKUP(R429,'ESO zone constants'!$E$3:$J$1002,5,FALSE),"")</f>
+        <v/>
+      </c>
       <c r="Y429" s="7" t="str">
         <f t="shared" si="30"/>
         <v/>
@@ -39398,7 +39689,11 @@
         <v/>
       </c>
     </row>
-    <row r="430" spans="17:29" x14ac:dyDescent="0.25">
+    <row r="430" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="Q430" s="3" t="str">
+        <f>IF(R430&lt;&gt;"",VLOOKUP(R430,'ESO zone constants'!$E$3:$J$1002,5,FALSE),"")</f>
+        <v/>
+      </c>
       <c r="Y430" s="7" t="str">
         <f t="shared" si="30"/>
         <v/>
@@ -39420,7 +39715,11 @@
         <v/>
       </c>
     </row>
-    <row r="431" spans="17:29" x14ac:dyDescent="0.25">
+    <row r="431" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="Q431" s="3" t="str">
+        <f>IF(R431&lt;&gt;"",VLOOKUP(R431,'ESO zone constants'!$E$3:$J$1002,5,FALSE),"")</f>
+        <v/>
+      </c>
       <c r="Y431" s="7" t="str">
         <f t="shared" si="30"/>
         <v/>
@@ -39442,7 +39741,11 @@
         <v/>
       </c>
     </row>
-    <row r="432" spans="17:29" x14ac:dyDescent="0.25">
+    <row r="432" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="Q432" s="3" t="str">
+        <f>IF(R432&lt;&gt;"",VLOOKUP(R432,'ESO zone constants'!$E$3:$J$1002,5,FALSE),"")</f>
+        <v/>
+      </c>
       <c r="Y432" s="7" t="str">
         <f t="shared" si="30"/>
         <v/>
@@ -39464,7 +39767,11 @@
         <v/>
       </c>
     </row>
-    <row r="433" spans="25:29" x14ac:dyDescent="0.25">
+    <row r="433" spans="17:29" x14ac:dyDescent="0.25">
+      <c r="Q433" s="3" t="str">
+        <f>IF(R433&lt;&gt;"",VLOOKUP(R433,'ESO zone constants'!$E$3:$J$1002,5,FALSE),"")</f>
+        <v/>
+      </c>
       <c r="Y433" s="7" t="str">
         <f t="shared" si="30"/>
         <v/>
@@ -39486,7 +39793,11 @@
         <v/>
       </c>
     </row>
-    <row r="434" spans="25:29" x14ac:dyDescent="0.25">
+    <row r="434" spans="17:29" x14ac:dyDescent="0.25">
+      <c r="Q434" s="3" t="str">
+        <f>IF(R434&lt;&gt;"",VLOOKUP(R434,'ESO zone constants'!$E$3:$J$1002,5,FALSE),"")</f>
+        <v/>
+      </c>
       <c r="Y434" s="7" t="str">
         <f t="shared" si="30"/>
         <v/>
@@ -39508,7 +39819,11 @@
         <v/>
       </c>
     </row>
-    <row r="435" spans="25:29" x14ac:dyDescent="0.25">
+    <row r="435" spans="17:29" x14ac:dyDescent="0.25">
+      <c r="Q435" s="3" t="str">
+        <f>IF(R435&lt;&gt;"",VLOOKUP(R435,'ESO zone constants'!$E$3:$J$1002,5,FALSE),"")</f>
+        <v/>
+      </c>
       <c r="Y435" s="7" t="str">
         <f t="shared" si="30"/>
         <v/>
@@ -39530,7 +39845,11 @@
         <v/>
       </c>
     </row>
-    <row r="436" spans="25:29" x14ac:dyDescent="0.25">
+    <row r="436" spans="17:29" x14ac:dyDescent="0.25">
+      <c r="Q436" s="3" t="str">
+        <f>IF(R436&lt;&gt;"",VLOOKUP(R436,'ESO zone constants'!$E$3:$J$1002,5,FALSE),"")</f>
+        <v/>
+      </c>
       <c r="Y436" s="7" t="str">
         <f t="shared" si="30"/>
         <v/>
@@ -39552,7 +39871,11 @@
         <v/>
       </c>
     </row>
-    <row r="437" spans="25:29" x14ac:dyDescent="0.25">
+    <row r="437" spans="17:29" x14ac:dyDescent="0.25">
+      <c r="Q437" s="3" t="str">
+        <f>IF(R437&lt;&gt;"",VLOOKUP(R437,'ESO zone constants'!$E$3:$J$1002,5,FALSE),"")</f>
+        <v/>
+      </c>
       <c r="Y437" s="7" t="str">
         <f t="shared" si="30"/>
         <v/>
@@ -39574,7 +39897,11 @@
         <v/>
       </c>
     </row>
-    <row r="438" spans="25:29" x14ac:dyDescent="0.25">
+    <row r="438" spans="17:29" x14ac:dyDescent="0.25">
+      <c r="Q438" s="3" t="str">
+        <f>IF(R438&lt;&gt;"",VLOOKUP(R438,'ESO zone constants'!$E$3:$J$1002,5,FALSE),"")</f>
+        <v/>
+      </c>
       <c r="Y438" s="7" t="str">
         <f t="shared" si="30"/>
         <v/>
@@ -39596,7 +39923,11 @@
         <v/>
       </c>
     </row>
-    <row r="439" spans="25:29" x14ac:dyDescent="0.25">
+    <row r="439" spans="17:29" x14ac:dyDescent="0.25">
+      <c r="Q439" s="3" t="str">
+        <f>IF(R439&lt;&gt;"",VLOOKUP(R439,'ESO zone constants'!$E$3:$J$1002,5,FALSE),"")</f>
+        <v/>
+      </c>
       <c r="Y439" s="7" t="str">
         <f t="shared" si="30"/>
         <v/>
@@ -39618,7 +39949,11 @@
         <v/>
       </c>
     </row>
-    <row r="440" spans="25:29" x14ac:dyDescent="0.25">
+    <row r="440" spans="17:29" x14ac:dyDescent="0.25">
+      <c r="Q440" s="3" t="str">
+        <f>IF(R440&lt;&gt;"",VLOOKUP(R440,'ESO zone constants'!$E$3:$J$1002,5,FALSE),"")</f>
+        <v/>
+      </c>
       <c r="Y440" s="7" t="str">
         <f t="shared" si="30"/>
         <v/>
@@ -39640,7 +39975,11 @@
         <v/>
       </c>
     </row>
-    <row r="441" spans="25:29" x14ac:dyDescent="0.25">
+    <row r="441" spans="17:29" x14ac:dyDescent="0.25">
+      <c r="Q441" s="3" t="str">
+        <f>IF(R441&lt;&gt;"",VLOOKUP(R441,'ESO zone constants'!$E$3:$J$1002,5,FALSE),"")</f>
+        <v/>
+      </c>
       <c r="Y441" s="7" t="str">
         <f t="shared" si="30"/>
         <v/>
@@ -39662,7 +40001,11 @@
         <v/>
       </c>
     </row>
-    <row r="442" spans="25:29" x14ac:dyDescent="0.25">
+    <row r="442" spans="17:29" x14ac:dyDescent="0.25">
+      <c r="Q442" s="3" t="str">
+        <f>IF(R442&lt;&gt;"",VLOOKUP(R442,'ESO zone constants'!$E$3:$J$1002,5,FALSE),"")</f>
+        <v/>
+      </c>
       <c r="Y442" s="7" t="str">
         <f t="shared" si="30"/>
         <v/>
@@ -39684,7 +40027,11 @@
         <v/>
       </c>
     </row>
-    <row r="443" spans="25:29" x14ac:dyDescent="0.25">
+    <row r="443" spans="17:29" x14ac:dyDescent="0.25">
+      <c r="Q443" s="3" t="str">
+        <f>IF(R443&lt;&gt;"",VLOOKUP(R443,'ESO zone constants'!$E$3:$J$1002,5,FALSE),"")</f>
+        <v/>
+      </c>
       <c r="Y443" s="7" t="str">
         <f t="shared" si="30"/>
         <v/>
@@ -39706,7 +40053,11 @@
         <v/>
       </c>
     </row>
-    <row r="444" spans="25:29" x14ac:dyDescent="0.25">
+    <row r="444" spans="17:29" x14ac:dyDescent="0.25">
+      <c r="Q444" s="3" t="str">
+        <f>IF(R444&lt;&gt;"",VLOOKUP(R444,'ESO zone constants'!$E$3:$J$1002,5,FALSE),"")</f>
+        <v/>
+      </c>
       <c r="Y444" s="7" t="str">
         <f t="shared" si="30"/>
         <v/>
@@ -39728,7 +40079,11 @@
         <v/>
       </c>
     </row>
-    <row r="445" spans="25:29" x14ac:dyDescent="0.25">
+    <row r="445" spans="17:29" x14ac:dyDescent="0.25">
+      <c r="Q445" s="3" t="str">
+        <f>IF(R445&lt;&gt;"",VLOOKUP(R445,'ESO zone constants'!$E$3:$J$1002,5,FALSE),"")</f>
+        <v/>
+      </c>
       <c r="Y445" s="7" t="str">
         <f t="shared" si="30"/>
         <v/>
@@ -39750,7 +40105,11 @@
         <v/>
       </c>
     </row>
-    <row r="446" spans="25:29" x14ac:dyDescent="0.25">
+    <row r="446" spans="17:29" x14ac:dyDescent="0.25">
+      <c r="Q446" s="3" t="str">
+        <f>IF(R446&lt;&gt;"",VLOOKUP(R446,'ESO zone constants'!$E$3:$J$1002,5,FALSE),"")</f>
+        <v/>
+      </c>
       <c r="Y446" s="7" t="str">
         <f t="shared" si="30"/>
         <v/>
@@ -39772,7 +40131,11 @@
         <v/>
       </c>
     </row>
-    <row r="447" spans="25:29" x14ac:dyDescent="0.25">
+    <row r="447" spans="17:29" x14ac:dyDescent="0.25">
+      <c r="Q447" s="3" t="str">
+        <f>IF(R447&lt;&gt;"",VLOOKUP(R447,'ESO zone constants'!$E$3:$J$1002,5,FALSE),"")</f>
+        <v/>
+      </c>
       <c r="Y447" s="7" t="str">
         <f t="shared" si="30"/>
         <v/>
@@ -39794,7 +40157,11 @@
         <v/>
       </c>
     </row>
-    <row r="448" spans="25:29" x14ac:dyDescent="0.25">
+    <row r="448" spans="17:29" x14ac:dyDescent="0.25">
+      <c r="Q448" s="3" t="str">
+        <f>IF(R448&lt;&gt;"",VLOOKUP(R448,'ESO zone constants'!$E$3:$J$1002,5,FALSE),"")</f>
+        <v/>
+      </c>
       <c r="Y448" s="7" t="str">
         <f t="shared" si="30"/>
         <v/>
@@ -40487,7 +40854,7 @@
   <dimension ref="A1:H90"/>
   <sheetViews>
     <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B90" sqref="B90"/>
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40503,7 +40870,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="23" t="s">
-        <v>2554</v>
+        <v>2553</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -42557,7 +42924,7 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>2555</v>
+        <v>2554</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>2548</v>
@@ -42585,7 +42952,7 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>2555</v>
+        <v>2554</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>2549</v>
@@ -42613,7 +42980,7 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>2555</v>
+        <v>2554</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>497</v>
@@ -42641,7 +43008,7 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>2555</v>
+        <v>2554</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>747</v>
@@ -42669,7 +43036,7 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>2555</v>
+        <v>2554</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>835</v>
@@ -42697,7 +43064,7 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>2555</v>
+        <v>2554</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>2550</v>
@@ -42725,7 +43092,7 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>2555</v>
+        <v>2554</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>1194</v>
@@ -42753,10 +43120,10 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>2555</v>
+        <v>2554</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>2552</v>
+        <v>2564</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>2551</v>
@@ -42781,7 +43148,7 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>2555</v>
+        <v>2554</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>2548</v>
@@ -42809,7 +43176,7 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>2555</v>
+        <v>2554</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>2549</v>
@@ -42837,7 +43204,7 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>2555</v>
+        <v>2554</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>497</v>
@@ -42865,7 +43232,7 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>2555</v>
+        <v>2554</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>747</v>
@@ -42893,7 +43260,7 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>2555</v>
+        <v>2554</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>835</v>
@@ -42921,7 +43288,7 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>2555</v>
+        <v>2554</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>2550</v>
@@ -42949,7 +43316,7 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>2555</v>
+        <v>2554</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>1194</v>
@@ -42977,10 +43344,10 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>2555</v>
+        <v>2554</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>2557</v>
+        <v>2564</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>2551</v>
@@ -43025,10 +43392,10 @@
   <dimension ref="A1:L718"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D207" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D547" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J221" sqref="J221"/>
+      <selection pane="bottomRight" activeCell="D563" sqref="D563"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43048,7 +43415,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="30" t="s">
-        <v>2556</v>
+        <v>2555</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
@@ -52037,13 +52404,13 @@
     </row>
     <row r="221" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A221" s="6" t="s">
-        <v>2553</v>
+        <v>2552</v>
       </c>
       <c r="B221" s="6" t="s">
-        <v>2553</v>
+        <v>2552</v>
       </c>
       <c r="C221" s="6" t="s">
-        <v>2553</v>
+        <v>2552</v>
       </c>
       <c r="D221" s="2" t="s">
         <v>1395</v>
@@ -66046,16 +66413,16 @@
     </row>
     <row r="563" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A563" s="27" t="s">
-        <v>2553</v>
+        <v>2552</v>
       </c>
       <c r="B563" s="27" t="s">
-        <v>2553</v>
+        <v>2552</v>
       </c>
       <c r="C563" s="27" t="s">
-        <v>2553</v>
+        <v>2552</v>
       </c>
       <c r="D563" s="28" t="s">
-        <v>2557</v>
+        <v>2564</v>
       </c>
       <c r="E563" s="28" t="s">
         <v>2551</v>

</xml_diff>